<commit_message>
feat: add new task
</commit_message>
<xml_diff>
--- a/bert-tasks.xlsx
+++ b/bert-tasks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/long/Library/CloudStorage/GoogleDrive-huulongpham28@gmail.com/マイドライブ/仕事/NTCIR19/Tasks/Pre-trained BERT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huulo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101DD0C7-1E3D-ED49-B661-3B6BF7244787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F65198A-B8EF-438C-B694-B87136F76031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="25600" windowHeight="26380" xr2:uid="{78A58A8E-D81B-3045-A71E-AB9604236B0F}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="23657" windowHeight="15120" xr2:uid="{78A58A8E-D81B-3045-A71E-AB9604236B0F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="101">
   <si>
     <t>emotion</t>
   </si>
@@ -271,10 +271,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>zefang-liu/phishing-email-dataset</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>raquiba/Sarcasm_News_Headline</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -393,6 +389,17 @@
   </si>
   <si>
     <t>verse_text</t>
+  </si>
+  <si>
+    <t>jackhhao/jailbreak-classification</t>
+  </si>
+  <si>
+    <t>prompt</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
@@ -806,35 +813,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B817599-7838-7348-80C1-B2DBFAA3A328}">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
-      <selection activeCell="N50" sqref="N50"/>
+    <sheetView tabSelected="1" topLeftCell="D33" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="19.3"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.4375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.5625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.125" customWidth="1"/>
+    <col min="4" max="4" width="17.5625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.7109375" style="1"/>
+    <col min="9" max="10" width="10.6875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" t="s">
         <v>88</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>89</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>90</v>
-      </c>
-      <c r="D1" t="s">
-        <v>91</v>
       </c>
       <c r="E1" t="s">
         <v>39</v>
@@ -846,22 +853,22 @@
         <v>40</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -1180,7 +1187,7 @@
         <v>4</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G9" t="s">
         <v>42</v>
@@ -1710,7 +1717,7 @@
         <v>2</v>
       </c>
       <c r="F24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G24" t="s">
         <v>42</v>
@@ -1887,7 +1894,7 @@
         <v>47</v>
       </c>
       <c r="G30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H30" s="1">
         <v>43400</v>
@@ -1924,7 +1931,7 @@
         <v>4</v>
       </c>
       <c r="F31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G31" t="s">
         <v>42</v>
@@ -1958,7 +1965,7 @@
         <v>4</v>
       </c>
       <c r="F32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G32" t="s">
         <v>50</v>
@@ -2122,7 +2129,7 @@
         <v>2</v>
       </c>
       <c r="F37" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G37" t="s">
         <v>42</v>
@@ -2146,7 +2153,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="3"/>
@@ -2156,7 +2163,7 @@
         <v>14</v>
       </c>
       <c r="F38" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G38" t="s">
         <v>42</v>
@@ -2190,7 +2197,7 @@
         <v>10</v>
       </c>
       <c r="F39" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G39" t="s">
         <v>50</v>
@@ -2408,26 +2415,32 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="3"/>
-        <v>https://huggingface.co/datasets/zefang-liu/phishing-email-dataset</v>
+        <v>https://huggingface.co/datasets/jackhhao/jailbreak-classification</v>
       </c>
       <c r="E45">
         <v>2</v>
       </c>
       <c r="F45" t="s">
-        <v>54</v>
+        <v>99</v>
       </c>
       <c r="G45" t="s">
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="H45" s="1">
-        <v>18700</v>
+        <v>1044</v>
+      </c>
+      <c r="J45" s="1">
+        <v>262</v>
       </c>
       <c r="K45" t="s">
         <v>32</v>
+      </c>
+      <c r="M45" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="46" spans="1:13">
@@ -2436,7 +2449,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="3"/>
@@ -2446,10 +2459,10 @@
         <v>2</v>
       </c>
       <c r="F46" t="s">
+        <v>68</v>
+      </c>
+      <c r="G46" t="s">
         <v>69</v>
-      </c>
-      <c r="G46" t="s">
-        <v>70</v>
       </c>
       <c r="H46" s="1">
         <v>28600</v>
@@ -2470,7 +2483,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C47" t="str">
         <f t="shared" si="3"/>
@@ -2483,7 +2496,7 @@
         <v>47</v>
       </c>
       <c r="G47" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H47" s="1">
         <v>200000</v>
@@ -2498,7 +2511,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C48" t="str">
         <f t="shared" si="3"/>
@@ -2511,7 +2524,7 @@
         <v>47</v>
       </c>
       <c r="G48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H48" s="1">
         <v>8000</v>
@@ -2532,7 +2545,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="3"/>
@@ -2545,7 +2558,7 @@
         <v>66</v>
       </c>
       <c r="G49" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H49" s="1">
         <v>32900</v>
@@ -2566,7 +2579,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="3"/>
@@ -2593,14 +2606,14 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="3"/>
         <v>https://huggingface.co/datasets/toxigen/toxigen-data</v>
       </c>
       <c r="D51" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E51">
         <v>5</v>
@@ -2609,7 +2622,7 @@
         <v>47</v>
       </c>
       <c r="G51" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H51" s="1">
         <v>8960</v>

</xml_diff>

<commit_message>
fix: remove test split from glue and sst2 due to no label
</commit_message>
<xml_diff>
--- a/bert-tasks.xlsx
+++ b/bert-tasks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huulo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/longpham28/Documents/GitHub/ntcir19-pretrained-model-retrieval/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F65198A-B8EF-438C-B694-B87136F76031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{062BCAC1-87D0-AB45-A875-5F6CDBB2A7A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="23657" windowHeight="15120" xr2:uid="{78A58A8E-D81B-3045-A71E-AB9604236B0F}"/>
+    <workbookView xWindow="0" yWindow="800" windowWidth="41120" windowHeight="25780" xr2:uid="{78A58A8E-D81B-3045-A71E-AB9604236B0F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="101">
   <si>
     <t>emotion</t>
   </si>
@@ -813,21 +813,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B817599-7838-7348-80C1-B2DBFAA3A328}">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D33" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="19.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="20"/>
   <cols>
-    <col min="1" max="1" width="6.4375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.5625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.125" customWidth="1"/>
-    <col min="4" max="4" width="17.5625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.6875" style="1"/>
+    <col min="9" max="10" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -1526,17 +1526,11 @@
       <c r="I18" s="1">
         <v>872</v>
       </c>
-      <c r="J18" s="1">
-        <v>1820</v>
-      </c>
       <c r="K18" t="s">
         <v>32</v>
       </c>
       <c r="L18" t="s">
         <v>60</v>
-      </c>
-      <c r="M18" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -2245,17 +2239,11 @@
       <c r="I40">
         <v>1040</v>
       </c>
-      <c r="J40" s="1">
-        <v>1060</v>
-      </c>
       <c r="K40" t="s">
         <v>32</v>
       </c>
       <c r="L40" t="s">
         <v>60</v>
-      </c>
-      <c r="M40" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:13">

</xml_diff>